<commit_message>
add Get Batch Feature
</commit_message>
<xml_diff>
--- a/src/test/resources/normal.xlsx
+++ b/src/test/resources/normal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romaindauvert/Projects/Tekhne/Projet-koala/eucalyptus-xls/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452E0D41-A8A4-394E-83D2-057628D1EB6D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BEC9B8-8420-C34A-9B6D-8BBDD5696E10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="25100" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>MORZINE</t>
   </si>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>LG</t>
-  </si>
-  <si>
-    <t>1234a</t>
   </si>
   <si>
     <t>Adresse 3</t>
@@ -692,8 +689,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -995,8 +992,8 @@
       <c r="E5" s="2">
         <v>1159</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>66</v>
+      <c r="F5" s="1">
+        <v>1234</v>
       </c>
       <c r="G5" s="1">
         <v>432</v>
@@ -1029,7 +1026,7 @@
         <v>7</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R5" s="1">
         <v>74110</v>

</xml_diff>

<commit_message>
Get batch feature (#7)
* update gitignore

* Batch persisted in mongo database

* start get batch feature

* Add service for fetching a batch from it's uid

todo:
[ ] Add Error management
[ ] Add missing batch case

* add Get Batch Feature
</commit_message>
<xml_diff>
--- a/src/test/resources/normal.xlsx
+++ b/src/test/resources/normal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romaindauvert/Projects/Tekhne/Projet-koala/eucalyptus-xls/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452E0D41-A8A4-394E-83D2-057628D1EB6D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BEC9B8-8420-C34A-9B6D-8BBDD5696E10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="25100" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>MORZINE</t>
   </si>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>LG</t>
-  </si>
-  <si>
-    <t>1234a</t>
   </si>
   <si>
     <t>Adresse 3</t>
@@ -692,8 +689,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -995,8 +992,8 @@
       <c r="E5" s="2">
         <v>1159</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>66</v>
+      <c r="F5" s="1">
+        <v>1234</v>
       </c>
       <c r="G5" s="1">
         <v>432</v>
@@ -1029,7 +1026,7 @@
         <v>7</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R5" s="1">
         <v>74110</v>

</xml_diff>